<commit_message>
Entrega 5 + Fichas Fantasna
</commit_message>
<xml_diff>
--- a/N1-FP-PROYECTO_v01.xlsx
+++ b/N1-FP-PROYECTO_v01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejaverianaedu-my.sharepoint.com/personal/crivera_javeriana_edu_co/Documents/Mojana control de archivos/REV_FICHAS/FICHAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="455" documentId="13_ncr:1_{2AC714FB-EBE8-4040-AC59-7C8A3337B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A5D5CD-24F9-47A8-8C1C-2CB24E7213D4}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:1_{2AC714FB-EBE8-4040-AC59-7C8A3337B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47FBF724-4158-4B96-80E5-2913C18EB642}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="954">
   <si>
     <t>Código de proyecto</t>
   </si>
@@ -1071,9 +1071,6 @@
   </si>
   <si>
     <t>12-Alternativas SM-MG</t>
-  </si>
-  <si>
-    <t>DEFINIR LAS OBRAS DE PROTECCIÓN ÓPTIMAS Y COSTO EFICIENTES PARA REDUCIR EL RIESGO POR INUNDACIÓN DE LOS CASCOS URBANOS DE LOS MUNICIPIOS DE SAN MARCOS (SUCRE) Y MAGANGUÉ (BOLÍVAR)</t>
   </si>
   <si>
     <t>Definir las obras de protección óptimas y costo eficientes para reducir el riesgo por inundación de los cascos urbanos de los municipios de San Marcos (Sucre) y Magangué (Bolívar)</t>
@@ -3407,7 +3404,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -3709,8 +3706,8 @@
   <dimension ref="A1:Y83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U69" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V82" sqref="V82"/>
+      <pane xSplit="2" topLeftCell="C15" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D19" sqref="D19"/>
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -5309,10 +5306,10 @@
         <v>292</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>293</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>294</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>29</v>
@@ -5327,7 +5324,7 @@
         <v>65</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>52</v>
@@ -5351,22 +5348,22 @@
         <v>9999</v>
       </c>
       <c r="R22" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="S22" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="S22" s="7" t="s">
+      <c r="T22" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="T22" s="7" t="s">
+      <c r="U22" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="U22" s="7" t="s">
+      <c r="V22" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="V22" s="7" t="s">
+      <c r="W22" s="7" t="s">
         <v>300</v>
-      </c>
-      <c r="W22" s="7" t="s">
-        <v>301</v>
       </c>
       <c r="X22" s="7" t="s">
         <v>275</v>
@@ -5374,19 +5371,19 @@
     </row>
     <row r="23" spans="1:24" customFormat="1">
       <c r="A23" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>306</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>29</v>
@@ -5401,16 +5398,16 @@
         <v>108</v>
       </c>
       <c r="J23" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M23" s="7" t="s">
         <v>307</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>308</v>
       </c>
       <c r="N23" s="8">
         <v>3846506245</v>
@@ -5425,22 +5422,22 @@
         <v>8</v>
       </c>
       <c r="R23" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="S23" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="S23" s="7" t="s">
+      <c r="T23" s="7" t="s">
         <v>310</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>311</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>233</v>
       </c>
       <c r="V23" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="W23" s="7" t="s">
         <v>312</v>
-      </c>
-      <c r="W23" s="7" t="s">
-        <v>313</v>
       </c>
       <c r="X23" s="7" t="s">
         <v>102</v>
@@ -5448,25 +5445,25 @@
     </row>
     <row r="24" spans="1:24" customFormat="1">
       <c r="A24" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="F24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>318</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>319</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>29</v>
@@ -5475,7 +5472,7 @@
         <v>108</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>52</v>
@@ -5500,7 +5497,7 @@
         <v>18</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="S24" s="7" t="s">
         <v>71</v>
@@ -5509,13 +5506,13 @@
         <v>98</v>
       </c>
       <c r="U24" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="V24" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="V24" s="7" t="s">
+      <c r="W24" s="7" t="s">
         <v>323</v>
-      </c>
-      <c r="W24" s="7" t="s">
-        <v>324</v>
       </c>
       <c r="X24" s="7" t="s">
         <v>102</v>
@@ -5523,13 +5520,13 @@
     </row>
     <row r="25" spans="1:24" customFormat="1">
       <c r="A25" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>326</v>
-      </c>
       <c r="C25" s="16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>52</v>
@@ -5574,33 +5571,33 @@
         <v>9999</v>
       </c>
       <c r="R25" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="S25" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="S25" s="12" t="s">
+      <c r="T25" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="T25" s="12" t="s">
+      <c r="U25" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="U25" s="16" t="s">
+      <c r="V25" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="V25" s="16" t="s">
+      <c r="W25" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="W25" s="16" t="s">
+      <c r="X25" s="16" t="s">
         <v>332</v>
-      </c>
-      <c r="X25" s="16" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>334</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>335</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>52</v>
@@ -5642,28 +5639,28 @@
         <v>9999</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q26" s="16">
         <v>9999</v>
       </c>
       <c r="R26" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="S26" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="S26" s="16" t="s">
+      <c r="T26" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="U26" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="T26" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="U26" s="16" t="s">
+      <c r="V26" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="V26" s="16" t="s">
+      <c r="W26" s="16" t="s">
         <v>340</v>
-      </c>
-      <c r="W26" s="16" t="s">
-        <v>341</v>
       </c>
       <c r="X26" s="16" t="s">
         <v>102</v>
@@ -5671,31 +5668,31 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="D27" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="16" t="s">
+      <c r="H27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="16" t="s">
         <v>347</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>348</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>268</v>
@@ -5718,22 +5715,22 @@
         <v>11</v>
       </c>
       <c r="R27" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="S27" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="S27" s="16" t="s">
+      <c r="T27" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="T27" s="16" t="s">
+      <c r="U27" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="U27" s="16" t="s">
+      <c r="V27" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="V27" s="16" t="s">
+      <c r="W27" s="16" t="s">
         <v>353</v>
-      </c>
-      <c r="W27" s="16" t="s">
-        <v>354</v>
       </c>
       <c r="X27" s="16" t="s">
         <v>289</v>
@@ -5741,46 +5738,46 @@
     </row>
     <row r="28" spans="1:24" s="34" customFormat="1">
       <c r="A28" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>355</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="C28" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="D28" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="E28" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="35" t="s">
         <v>358</v>
       </c>
-      <c r="E28" s="35" t="s">
-        <v>356</v>
-      </c>
-      <c r="F28" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G28" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="35" t="s">
+      <c r="I28" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="I28" s="35" t="s">
+      <c r="J28" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="J28" s="35" t="s">
+      <c r="K28" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="M28" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="K28" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="L28" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="M28" s="35" t="s">
+      <c r="N28" s="38" t="s">
         <v>362</v>
-      </c>
-      <c r="N28" s="38" t="s">
-        <v>363</v>
       </c>
       <c r="O28" s="39">
         <v>41340</v>
@@ -5792,39 +5789,39 @@
         <v>4</v>
       </c>
       <c r="R28" s="35" t="s">
+        <v>363</v>
+      </c>
+      <c r="S28" s="35" t="s">
         <v>364</v>
       </c>
-      <c r="S28" s="35" t="s">
+      <c r="T28" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="U28" s="35" t="s">
         <v>365</v>
       </c>
-      <c r="T28" s="35" t="s">
-        <v>365</v>
-      </c>
-      <c r="U28" s="35" t="s">
+      <c r="V28" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="V28" s="35" t="s">
+      <c r="W28" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="W28" s="35" t="s">
+      <c r="X28" s="35" t="s">
         <v>368</v>
-      </c>
-      <c r="X28" s="35" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:24">
       <c r="A29" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>372</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>373</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>171</v>
@@ -5875,13 +5872,13 @@
         <v>176</v>
       </c>
       <c r="U29" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="V29" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="V29" s="7" t="s">
+      <c r="W29" s="7" t="s">
         <v>375</v>
-      </c>
-      <c r="W29" s="7" t="s">
-        <v>376</v>
       </c>
       <c r="X29" s="7" t="s">
         <v>153</v>
@@ -5889,43 +5886,43 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="E30" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="H30" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="J30" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="K30" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="K30" s="7" t="s">
-        <v>385</v>
-      </c>
       <c r="L30" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="N30" s="23">
         <v>253146213</v>
@@ -5940,30 +5937,30 @@
         <v>12</v>
       </c>
       <c r="R30" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="S30" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="S30" s="7" t="s">
+      <c r="T30" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="T30" s="7" t="s">
+      <c r="U30" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="U30" s="7" t="s">
+      <c r="V30" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="V30" s="7" t="s">
+      <c r="W30" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="W30" s="7" t="s">
-        <v>391</v>
-      </c>
       <c r="X30" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="A31" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>182</v>
@@ -5972,7 +5969,7 @@
         <v>183</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>185</v>
@@ -5990,7 +5987,7 @@
         <v>65</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>52</v>
@@ -6005,16 +6002,16 @@
         <v>2734719994</v>
       </c>
       <c r="O31" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="P31" s="9" t="s">
         <v>395</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>396</v>
       </c>
       <c r="Q31" s="7">
         <v>7</v>
       </c>
       <c r="R31" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S31" s="7" t="s">
         <v>71</v>
@@ -6023,57 +6020,57 @@
         <v>98</v>
       </c>
       <c r="U31" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="V31" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="V31" s="7" t="s">
+      <c r="W31" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="W31" s="7" t="s">
+      <c r="X31" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="X31" s="7" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="32" spans="1:24">
       <c r="A32" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="C32" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>403</v>
-      </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>405</v>
-      </c>
       <c r="F32" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>65</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="N32" s="23">
         <v>216000000</v>
@@ -6088,39 +6085,39 @@
         <v>14</v>
       </c>
       <c r="R32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="V32" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="W32" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="W32" s="7" t="s">
+      <c r="X32" s="7" t="s">
         <v>408</v>
-      </c>
-      <c r="X32" s="7" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B33" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="C33" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
         <v>412</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>413</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>29</v>
@@ -6138,7 +6135,7 @@
         <v>65</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>52</v>
@@ -6153,31 +6150,31 @@
         <v>20901990031.84</v>
       </c>
       <c r="O33" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="P33" s="9" t="s">
         <v>415</v>
-      </c>
-      <c r="P33" s="9" t="s">
-        <v>416</v>
       </c>
       <c r="Q33" s="7">
         <v>11</v>
       </c>
       <c r="R33" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="S33" s="7" t="s">
         <v>417</v>
-      </c>
-      <c r="S33" s="7" t="s">
-        <v>418</v>
       </c>
       <c r="T33" s="18" t="s">
         <v>98</v>
       </c>
       <c r="U33" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="V33" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="V33" s="7" t="s">
+      <c r="W33" s="7" t="s">
         <v>420</v>
-      </c>
-      <c r="W33" s="7" t="s">
-        <v>421</v>
       </c>
       <c r="X33" s="7" t="s">
         <v>29</v>
@@ -6185,19 +6182,19 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>425</v>
-      </c>
       <c r="E34" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>29</v>
@@ -6212,7 +6209,7 @@
         <v>65</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>52</v>
@@ -6230,28 +6227,28 @@
         <v>138</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Q34" s="7">
         <v>10</v>
       </c>
       <c r="R34" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="T34" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="S34" s="7" t="s">
+      <c r="U34" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="T34" s="7" t="s">
+      <c r="V34" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="U34" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="V34" s="7" t="s">
+      <c r="W34" s="7" t="s">
         <v>430</v>
-      </c>
-      <c r="W34" s="7" t="s">
-        <v>431</v>
       </c>
       <c r="X34" s="7" t="s">
         <v>29</v>
@@ -6259,10 +6256,10 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>432</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>433</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>156</v>
@@ -6310,7 +6307,7 @@
         <v>6</v>
       </c>
       <c r="R35" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>163</v>
@@ -6325,7 +6322,7 @@
         <v>165</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="X35" s="7" t="s">
         <v>29</v>
@@ -6333,13 +6330,13 @@
     </row>
     <row r="36" spans="1:25" s="34" customFormat="1" ht="20.25" customHeight="1">
       <c r="A36" s="35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>213</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D36" s="35" t="s">
         <v>215</v>
@@ -6351,13 +6348,13 @@
         <v>29</v>
       </c>
       <c r="G36" s="35" t="s">
+        <v>437</v>
+      </c>
+      <c r="H36" s="35" t="s">
         <v>438</v>
       </c>
-      <c r="H36" s="35" t="s">
-        <v>439</v>
-      </c>
       <c r="I36" s="35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J36" s="35" t="s">
         <v>219</v>
@@ -6384,7 +6381,7 @@
         <v>67</v>
       </c>
       <c r="R36" s="41" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="S36" s="35" t="s">
         <v>71</v>
@@ -6393,33 +6390,33 @@
         <v>98</v>
       </c>
       <c r="U36" s="35" t="s">
+        <v>440</v>
+      </c>
+      <c r="V36" s="35" t="s">
         <v>441</v>
       </c>
-      <c r="V36" s="35" t="s">
+      <c r="W36" s="35" t="s">
         <v>442</v>
       </c>
-      <c r="W36" s="35" t="s">
-        <v>443</v>
-      </c>
       <c r="X36" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:25" s="34" customFormat="1">
       <c r="A37" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="B37" s="35" t="s">
         <v>444</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="C37" s="35" t="s">
         <v>445</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="D37" s="35" t="s">
         <v>446</v>
       </c>
-      <c r="D37" s="35" t="s">
-        <v>447</v>
-      </c>
       <c r="E37" s="35" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F37" s="35" t="s">
         <v>29</v>
@@ -6434,7 +6431,7 @@
         <v>65</v>
       </c>
       <c r="J37" s="35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K37" s="35" t="s">
         <v>52</v>
@@ -6458,36 +6455,36 @@
         <v>15</v>
       </c>
       <c r="R37" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="S37" s="35" t="s">
         <v>448</v>
-      </c>
-      <c r="S37" s="35" t="s">
-        <v>449</v>
       </c>
       <c r="T37" s="35" t="s">
         <v>98</v>
       </c>
       <c r="U37" s="35" t="s">
+        <v>449</v>
+      </c>
+      <c r="V37" s="35" t="s">
         <v>450</v>
       </c>
-      <c r="V37" s="35" t="s">
+      <c r="W37" s="35" t="s">
         <v>451</v>
       </c>
-      <c r="W37" s="35" t="s">
-        <v>452</v>
-      </c>
       <c r="X37" s="35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:25">
       <c r="A38" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>453</v>
       </c>
-      <c r="B38" s="16" t="s">
-        <v>454</v>
-      </c>
       <c r="C38" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>52</v>
@@ -6532,7 +6529,7 @@
         <v>9999</v>
       </c>
       <c r="R38" s="16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="S38" s="16" t="s">
         <v>163</v>
@@ -6541,24 +6538,24 @@
         <v>98</v>
       </c>
       <c r="U38" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="V38" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="V38" s="16" t="s">
+      <c r="W38" s="16" t="s">
         <v>457</v>
       </c>
-      <c r="W38" s="16" t="s">
-        <v>458</v>
-      </c>
       <c r="X38" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="39" spans="1:25">
       <c r="A39" s="25" t="s">
+        <v>458</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>459</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>460</v>
       </c>
       <c r="C39" s="25" t="s">
         <v>52</v>
@@ -6606,22 +6603,22 @@
         <v>9999</v>
       </c>
       <c r="R39" s="25" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="S39" s="25" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="T39" s="25" t="s">
         <v>98</v>
       </c>
       <c r="U39" s="25" t="s">
+        <v>461</v>
+      </c>
+      <c r="V39" s="25" t="s">
         <v>462</v>
       </c>
-      <c r="V39" s="25" t="s">
+      <c r="W39" s="25" t="s">
         <v>463</v>
-      </c>
-      <c r="W39" s="25" t="s">
-        <v>464</v>
       </c>
       <c r="X39" s="25" t="s">
         <v>275</v>
@@ -6629,13 +6626,13 @@
     </row>
     <row r="40" spans="1:25">
       <c r="A40" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>466</v>
-      </c>
       <c r="C40" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>52</v>
@@ -6680,49 +6677,49 @@
         <v>9999</v>
       </c>
       <c r="R40" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="S40" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T40" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="U40" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="S40" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="U40" s="7" t="s">
+      <c r="V40" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="V40" s="7" t="s">
+      <c r="W40" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="W40" s="7" t="s">
+      <c r="X40" s="7" t="s">
         <v>470</v>
-      </c>
-      <c r="X40" s="7" t="s">
-        <v>471</v>
       </c>
       <c r="Y40" s="16"/>
     </row>
     <row r="41" spans="1:25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>472</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="C41" s="16" t="s">
         <v>473</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="D41" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="E41" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="16" t="s">
         <v>475</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F41" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="16" t="s">
-        <v>476</v>
       </c>
       <c r="H41" s="16" t="s">
         <v>52</v>
@@ -6731,22 +6728,22 @@
         <v>65</v>
       </c>
       <c r="J41" s="16" t="s">
+        <v>476</v>
+      </c>
+      <c r="K41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M41" s="16" t="s">
         <v>477</v>
-      </c>
-      <c r="K41" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L41" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M41" s="16" t="s">
-        <v>478</v>
       </c>
       <c r="N41" s="22">
         <v>7578039678</v>
       </c>
       <c r="O41" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P41" s="12">
         <v>43499</v>
@@ -6755,58 +6752,58 @@
         <v>54</v>
       </c>
       <c r="R41" s="16" t="s">
+        <v>479</v>
+      </c>
+      <c r="S41" s="16" t="s">
         <v>480</v>
       </c>
-      <c r="S41" s="16" t="s">
+      <c r="T41" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="U41" s="16" t="s">
         <v>481</v>
       </c>
-      <c r="T41" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="U41" s="16" t="s">
+      <c r="V41" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="V41" s="16" t="s">
+      <c r="W41" s="16" t="s">
         <v>483</v>
       </c>
-      <c r="W41" s="16" t="s">
-        <v>484</v>
-      </c>
       <c r="X41" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Y41" s="1"/>
     </row>
     <row r="42" spans="1:25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="16" t="s">
+        <v>484</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>485</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="C42" s="16" t="s">
         <v>486</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="D42" s="16" t="s">
         <v>487</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="E42" s="16" t="s">
         <v>488</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="F42" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42" s="16" t="s">
         <v>489</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" s="16" t="s">
+      <c r="J42" s="16" t="s">
         <v>490</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>491</v>
       </c>
       <c r="K42" s="16" t="s">
         <v>52</v>
@@ -6821,74 +6818,74 @@
         <v>6471757378</v>
       </c>
       <c r="O42" s="22" t="s">
+        <v>491</v>
+      </c>
+      <c r="P42" s="12" t="s">
         <v>492</v>
-      </c>
-      <c r="P42" s="12" t="s">
-        <v>493</v>
       </c>
       <c r="Q42" s="16">
         <f>3*12+10</f>
         <v>46</v>
       </c>
       <c r="R42" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="S42" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="S42" s="16" t="s">
+      <c r="T42" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="T42" s="16" t="s">
+      <c r="U42" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="U42" s="16" t="s">
+      <c r="V42" s="16" t="s">
         <v>497</v>
       </c>
-      <c r="V42" s="16" t="s">
+      <c r="W42" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="W42" s="16" t="s">
+      <c r="X42" s="16" t="s">
         <v>499</v>
-      </c>
-      <c r="X42" s="16" t="s">
-        <v>500</v>
       </c>
       <c r="Y42" s="1"/>
     </row>
     <row r="43" spans="1:25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G43" s="7" t="s">
+      <c r="H43" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="H43" s="7" t="s">
-        <v>506</v>
-      </c>
-      <c r="I43" s="7" t="s">
+      <c r="J43" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="J43" s="7" t="s">
-        <v>508</v>
-      </c>
       <c r="K43" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="M43" s="7" t="s">
         <v>95</v>
@@ -6906,95 +6903,95 @@
         <v>9999</v>
       </c>
       <c r="R43" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="S43" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="S43" s="7" t="s">
+      <c r="T43" s="7" t="s">
         <v>510</v>
-      </c>
-      <c r="T43" s="7" t="s">
-        <v>511</v>
       </c>
       <c r="U43" s="7" t="s">
         <v>95</v>
       </c>
       <c r="V43" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="W43" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="W43" s="7" t="s">
+      <c r="X43" s="7" t="s">
         <v>513</v>
-      </c>
-      <c r="X43" s="7" t="s">
-        <v>514</v>
       </c>
       <c r="Y43" s="7"/>
     </row>
     <row r="44" spans="1:25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A44" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>517</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="E44" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>518</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>517</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>519</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="J44" s="7" t="s">
         <v>520</v>
       </c>
-      <c r="J44" s="7" t="s">
+      <c r="K44" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M44" s="7" t="s">
         <v>521</v>
-      </c>
-      <c r="K44" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L44" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="M44" s="7" t="s">
-        <v>522</v>
       </c>
       <c r="N44" s="8">
         <v>6514587989</v>
       </c>
       <c r="O44" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="P44" s="9" t="s">
         <v>523</v>
-      </c>
-      <c r="P44" s="9" t="s">
-        <v>524</v>
       </c>
       <c r="Q44" s="7">
         <v>60</v>
       </c>
       <c r="R44" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="S44" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="S44" s="7" t="s">
+      <c r="T44" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="T44" s="7" t="s">
+      <c r="U44" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="U44" s="7" t="s">
+      <c r="V44" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="V44" s="7" t="s">
+      <c r="W44" s="7" t="s">
         <v>529</v>
-      </c>
-      <c r="W44" s="7" t="s">
-        <v>530</v>
       </c>
       <c r="X44" s="7" t="s">
         <v>275</v>
@@ -7003,19 +7000,19 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="B45" s="16" t="s">
         <v>531</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="C45" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="D45" s="16" t="s">
         <v>533</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="E45" s="16" t="s">
         <v>534</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>535</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>29</v>
@@ -7063,39 +7060,39 @@
         <v>98</v>
       </c>
       <c r="U45" s="16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="V45" s="7" t="s">
         <v>129</v>
       </c>
       <c r="W45" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="X45" s="16" t="s">
         <v>537</v>
-      </c>
-      <c r="X45" s="16" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>539</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="E46" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="7" t="s">
         <v>542</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>543</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>29</v>
@@ -7104,7 +7101,7 @@
         <v>65</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K46" s="7" t="s">
         <v>29</v>
@@ -7128,22 +7125,22 @@
         <v>9999</v>
       </c>
       <c r="R46" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="S46" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="S46" s="7" t="s">
+      <c r="T46" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="U46" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="V46" s="7" t="s">
         <v>546</v>
       </c>
-      <c r="T46" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="U46" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="V46" s="7" t="s">
+      <c r="W46" s="7" t="s">
         <v>547</v>
-      </c>
-      <c r="W46" s="7" t="s">
-        <v>548</v>
       </c>
       <c r="X46" s="7" t="s">
         <v>275</v>
@@ -7151,25 +7148,25 @@
     </row>
     <row r="47" spans="1:25">
       <c r="A47" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C47" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>551</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>552</v>
-      </c>
       <c r="F47" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>29</v>
@@ -7178,16 +7175,16 @@
         <v>65</v>
       </c>
       <c r="J47" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M47" s="7" t="s">
         <v>553</v>
-      </c>
-      <c r="K47" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L47" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M47" s="7" t="s">
-        <v>554</v>
       </c>
       <c r="N47" s="8">
         <v>1837306186</v>
@@ -7202,22 +7199,22 @@
         <v>16.5</v>
       </c>
       <c r="R47" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="S47" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="S47" s="7" t="s">
+      <c r="T47" s="7" t="s">
         <v>556</v>
       </c>
-      <c r="T47" s="7" t="s">
+      <c r="U47" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="V47" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="U47" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="V47" s="7" t="s">
+      <c r="W47" s="7" t="s">
         <v>558</v>
-      </c>
-      <c r="W47" s="7" t="s">
-        <v>559</v>
       </c>
       <c r="X47" s="7" t="s">
         <v>275</v>
@@ -7225,25 +7222,25 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" s="16" t="s">
+        <v>559</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="C48" s="16" t="s">
         <v>561</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="D48" s="16" t="s">
         <v>562</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="E48" s="16" t="s">
         <v>563</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" s="16" t="s">
         <v>564</v>
-      </c>
-      <c r="F48" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>565</v>
       </c>
       <c r="H48" s="16" t="s">
         <v>29</v>
@@ -7252,16 +7249,16 @@
         <v>65</v>
       </c>
       <c r="J48" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="K48" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="K48" s="16" t="s">
+      <c r="L48" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M48" s="16" t="s">
         <v>567</v>
-      </c>
-      <c r="L48" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M48" s="16" t="s">
-        <v>568</v>
       </c>
       <c r="N48" s="22">
         <v>2066969459</v>
@@ -7276,22 +7273,22 @@
         <v>15</v>
       </c>
       <c r="R48" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="S48" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="S48" s="16" t="s">
+      <c r="T48" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="T48" s="16" t="s">
+      <c r="U48" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="U48" s="16" t="s">
+      <c r="V48" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="V48" s="16" t="s">
+      <c r="W48" s="16" t="s">
         <v>573</v>
-      </c>
-      <c r="W48" s="16" t="s">
-        <v>574</v>
       </c>
       <c r="X48" s="16" t="s">
         <v>275</v>
@@ -7299,17 +7296,17 @@
     </row>
     <row r="49" spans="1:24">
       <c r="A49" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>575</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>576</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>578</v>
-      </c>
       <c r="E49" s="7" t="s">
         <v>52</v>
       </c>
@@ -7317,7 +7314,7 @@
         <v>29</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>29</v>
@@ -7326,7 +7323,7 @@
         <v>65</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K49" s="7" t="s">
         <v>29</v>
@@ -7350,22 +7347,22 @@
         <v>9999</v>
       </c>
       <c r="R49" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="S49" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="S49" s="7" t="s">
+      <c r="T49" s="7" t="s">
         <v>581</v>
       </c>
-      <c r="T49" s="7" t="s">
+      <c r="U49" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="V49" s="7" t="s">
         <v>582</v>
       </c>
-      <c r="U49" s="7" t="s">
-        <v>528</v>
-      </c>
-      <c r="V49" s="7" t="s">
+      <c r="W49" s="7" t="s">
         <v>583</v>
-      </c>
-      <c r="W49" s="7" t="s">
-        <v>584</v>
       </c>
       <c r="X49" s="7" t="s">
         <v>275</v>
@@ -7373,34 +7370,34 @@
     </row>
     <row r="50" spans="1:24" ht="18.75" customHeight="1">
       <c r="A50" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="B50" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="C50" s="16" t="s">
         <v>586</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="D50" s="16" t="s">
         <v>587</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="E50" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G50" s="16" t="s">
         <v>588</v>
       </c>
-      <c r="E50" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G50" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>589</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>590</v>
       </c>
       <c r="I50" s="16" t="s">
         <v>65</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K50" s="16" t="s">
         <v>52</v>
@@ -7424,51 +7421,51 @@
         <v>9999</v>
       </c>
       <c r="R50" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="S50" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="S50" s="16" t="s">
+      <c r="T50" s="16" t="s">
         <v>592</v>
       </c>
-      <c r="T50" s="16" t="s">
+      <c r="U50" s="29" t="s">
         <v>593</v>
       </c>
-      <c r="U50" s="29" t="s">
+      <c r="V50" s="16" t="s">
         <v>594</v>
       </c>
-      <c r="V50" s="16" t="s">
+      <c r="W50" s="16" t="s">
         <v>595</v>
       </c>
-      <c r="W50" s="16" t="s">
+      <c r="X50" s="29" t="s">
         <v>596</v>
-      </c>
-      <c r="X50" s="29" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="51" spans="1:24" ht="18.75" customHeight="1">
       <c r="A51" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="B51" s="16" t="s">
         <v>598</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="C51" s="29" t="s">
         <v>599</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="D51" s="16" t="s">
+        <v>599</v>
+      </c>
+      <c r="E51" s="16" t="s">
         <v>600</v>
       </c>
-      <c r="D51" s="16" t="s">
-        <v>600</v>
-      </c>
-      <c r="E51" s="16" t="s">
+      <c r="F51" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" s="29" t="s">
         <v>601</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H51" s="29" t="s">
-        <v>602</v>
       </c>
       <c r="I51" s="16" t="s">
         <v>65</v>
@@ -7492,13 +7489,13 @@
         <v>29</v>
       </c>
       <c r="P51" s="12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="Q51" s="16">
         <v>24</v>
       </c>
       <c r="R51" s="16" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="S51" s="16" t="s">
         <v>87</v>
@@ -7507,33 +7504,33 @@
         <v>98</v>
       </c>
       <c r="U51" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="V51" s="29" t="s">
         <v>605</v>
       </c>
-      <c r="V51" s="29" t="s">
+      <c r="W51" s="16" t="s">
         <v>606</v>
       </c>
-      <c r="W51" s="16" t="s">
+      <c r="X51" s="29" t="s">
         <v>607</v>
-      </c>
-      <c r="X51" s="29" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="52" spans="1:24">
       <c r="A52" s="16" t="s">
+        <v>608</v>
+      </c>
+      <c r="B52" s="16" t="s">
         <v>609</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="C52" s="16" t="s">
         <v>610</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="D52" s="16" t="s">
         <v>611</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="E52" s="16" t="s">
         <v>612</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>613</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>29</v>
@@ -7548,7 +7545,7 @@
         <v>108</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K52" s="16" t="s">
         <v>52</v>
@@ -7566,28 +7563,28 @@
         <v>43899</v>
       </c>
       <c r="P52" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q52" s="16" t="s">
         <v>615</v>
       </c>
-      <c r="Q52" s="16" t="s">
+      <c r="R52" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="R52" s="16" t="s">
+      <c r="S52" s="16" t="s">
         <v>617</v>
       </c>
-      <c r="S52" s="16" t="s">
+      <c r="T52" s="16" t="s">
+        <v>617</v>
+      </c>
+      <c r="U52" s="16" t="s">
         <v>618</v>
       </c>
-      <c r="T52" s="16" t="s">
-        <v>618</v>
-      </c>
-      <c r="U52" s="16" t="s">
+      <c r="V52" s="16" t="s">
         <v>619</v>
       </c>
-      <c r="V52" s="16" t="s">
+      <c r="W52" s="16" t="s">
         <v>620</v>
-      </c>
-      <c r="W52" s="16" t="s">
-        <v>621</v>
       </c>
       <c r="X52" s="16" t="s">
         <v>102</v>
@@ -7595,19 +7592,19 @@
     </row>
     <row r="53" spans="1:24">
       <c r="A53" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="B53" s="16" t="s">
         <v>622</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="C53" s="16" t="s">
         <v>623</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="D53" s="16" t="s">
         <v>624</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="E53" s="16" t="s">
         <v>625</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>626</v>
       </c>
       <c r="F53" s="16">
         <v>9999</v>
@@ -7622,7 +7619,7 @@
         <v>65</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K53" s="16" t="s">
         <v>52</v>
@@ -7640,48 +7637,48 @@
         <v>138</v>
       </c>
       <c r="P53" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Q53" s="16">
         <v>10</v>
       </c>
       <c r="R53" s="16" t="s">
+        <v>626</v>
+      </c>
+      <c r="S53" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="T53" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="U53" s="16" t="s">
         <v>627</v>
       </c>
-      <c r="S53" s="16" t="s">
-        <v>418</v>
-      </c>
-      <c r="T53" s="16" t="s">
-        <v>429</v>
-      </c>
-      <c r="U53" s="16" t="s">
+      <c r="V53" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="V53" s="16" t="s">
+      <c r="W53" s="16" t="s">
         <v>629</v>
       </c>
-      <c r="W53" s="16" t="s">
-        <v>630</v>
-      </c>
       <c r="X53" s="16" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="14.25" customHeight="1">
       <c r="A54" s="16" t="s">
+        <v>630</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>631</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="C54" s="16" t="s">
         <v>632</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="D54" s="16" t="s">
         <v>633</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="E54" s="16" t="s">
         <v>634</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>635</v>
       </c>
       <c r="F54" s="16" t="s">
         <v>29</v>
@@ -7690,66 +7687,66 @@
         <v>136</v>
       </c>
       <c r="H54" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="I54" s="16" t="s">
         <v>636</v>
-      </c>
-      <c r="I54" s="16" t="s">
-        <v>637</v>
       </c>
       <c r="J54" s="16" t="s">
         <v>65</v>
       </c>
       <c r="K54" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="L54" s="16" t="s">
         <v>638</v>
       </c>
-      <c r="L54" s="16" t="s">
+      <c r="M54" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N54" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="O54" s="12" t="s">
         <v>639</v>
       </c>
-      <c r="M54" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="N54" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="O54" s="12" t="s">
+      <c r="P54" s="3" t="s">
         <v>640</v>
-      </c>
-      <c r="P54" s="3" t="s">
-        <v>641</v>
       </c>
       <c r="Q54" s="16">
         <v>18</v>
       </c>
       <c r="R54" s="16" t="s">
+        <v>641</v>
+      </c>
+      <c r="S54" s="16" t="s">
         <v>642</v>
-      </c>
-      <c r="S54" s="16" t="s">
-        <v>643</v>
       </c>
       <c r="T54" s="16" t="s">
         <v>98</v>
       </c>
       <c r="U54" s="16" t="s">
+        <v>643</v>
+      </c>
+      <c r="V54" s="16" t="s">
         <v>644</v>
       </c>
-      <c r="V54" s="16" t="s">
+      <c r="W54" s="16" t="s">
         <v>645</v>
       </c>
-      <c r="W54" s="16" t="s">
-        <v>646</v>
-      </c>
       <c r="X54" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" spans="1:24">
       <c r="A55" s="16" t="s">
+        <v>646</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>647</v>
       </c>
-      <c r="B55" s="16" t="s">
-        <v>648</v>
-      </c>
       <c r="C55" s="16" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D55" s="16">
         <v>9999</v>
@@ -7767,10 +7764,10 @@
         <v>9999</v>
       </c>
       <c r="I55" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J55" s="16" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="K55" s="16" t="s">
         <v>52</v>
@@ -7794,63 +7791,63 @@
         <v>9999</v>
       </c>
       <c r="R55" s="16" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="S55" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="T55" s="16" t="s">
         <v>98</v>
       </c>
       <c r="U55" s="16" t="s">
+        <v>649</v>
+      </c>
+      <c r="V55" s="16" t="s">
         <v>650</v>
       </c>
-      <c r="V55" s="16" t="s">
+      <c r="W55" s="16" t="s">
         <v>651</v>
       </c>
-      <c r="W55" s="16" t="s">
-        <v>652</v>
-      </c>
       <c r="X55" s="16" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="56" spans="1:24">
       <c r="A56" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="B56" s="7" t="s">
         <v>653</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="D56" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I56" s="7" t="s">
         <v>655</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I56" s="7" t="s">
+      <c r="J56" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="J56" s="7" t="s">
+      <c r="K56" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="K56" s="7" t="s">
+      <c r="L56" s="7" t="s">
         <v>658</v>
-      </c>
-      <c r="L56" s="7" t="s">
-        <v>659</v>
       </c>
       <c r="M56" s="7" t="s">
         <v>29</v>
@@ -7862,28 +7859,28 @@
         <v>40186</v>
       </c>
       <c r="P56" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="Q56" s="7">
         <v>9999</v>
       </c>
       <c r="R56" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="S56" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="S56" s="7" t="s">
+      <c r="T56" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="U56" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="T56" s="7" t="s">
-        <v>662</v>
-      </c>
-      <c r="U56" s="7" t="s">
+      <c r="V56" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="V56" s="7" t="s">
+      <c r="W56" s="7" t="s">
         <v>664</v>
-      </c>
-      <c r="W56" s="7" t="s">
-        <v>665</v>
       </c>
       <c r="X56" s="7" t="s">
         <v>275</v>
@@ -7891,31 +7888,31 @@
     </row>
     <row r="57" spans="1:24">
       <c r="A57" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>666</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="C57" s="16" t="s">
         <v>667</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="D57" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I57" s="16" t="s">
         <v>668</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I57" s="16" t="s">
-        <v>669</v>
       </c>
       <c r="J57" s="16" t="s">
         <v>65</v>
@@ -7936,39 +7933,39 @@
         <v>45327</v>
       </c>
       <c r="P57" s="12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="Q57" s="16">
         <v>9999</v>
       </c>
       <c r="R57" s="16" t="s">
+        <v>670</v>
+      </c>
+      <c r="S57" s="16" t="s">
         <v>671</v>
-      </c>
-      <c r="S57" s="16" t="s">
-        <v>672</v>
       </c>
       <c r="T57" s="16" t="s">
         <v>98</v>
       </c>
       <c r="U57" s="16" t="s">
+        <v>672</v>
+      </c>
+      <c r="V57" s="16" t="s">
         <v>673</v>
       </c>
-      <c r="V57" s="16" t="s">
+      <c r="W57" s="16" t="s">
         <v>674</v>
       </c>
-      <c r="W57" s="16" t="s">
-        <v>675</v>
-      </c>
       <c r="X57" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="58" spans="1:24">
       <c r="A58" s="16" t="s">
+        <v>675</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>676</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>677</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>52</v>
@@ -8016,22 +8013,22 @@
         <v>9999</v>
       </c>
       <c r="R58" s="16" t="s">
+        <v>677</v>
+      </c>
+      <c r="S58" s="16" t="s">
+        <v>617</v>
+      </c>
+      <c r="T58" s="16" t="s">
+        <v>617</v>
+      </c>
+      <c r="U58" s="16" t="s">
         <v>678</v>
       </c>
-      <c r="S58" s="16" t="s">
-        <v>618</v>
-      </c>
-      <c r="T58" s="16" t="s">
-        <v>618</v>
-      </c>
-      <c r="U58" s="16" t="s">
+      <c r="V58" s="16" t="s">
         <v>679</v>
       </c>
-      <c r="V58" s="16" t="s">
+      <c r="W58" s="16" t="s">
         <v>680</v>
-      </c>
-      <c r="W58" s="16" t="s">
-        <v>681</v>
       </c>
       <c r="X58" s="16" t="s">
         <v>275</v>
@@ -8039,34 +8036,34 @@
     </row>
     <row r="59" spans="1:24">
       <c r="A59" s="16" t="s">
+        <v>681</v>
+      </c>
+      <c r="B59" s="16" t="s">
         <v>682</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="C59" s="16" t="s">
+        <v>682</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J59" s="16" t="s">
         <v>683</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>683</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I59" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>684</v>
       </c>
       <c r="K59" s="16" t="s">
         <v>52</v>
@@ -8090,48 +8087,48 @@
         <v>9999</v>
       </c>
       <c r="R59" s="16" t="s">
+        <v>684</v>
+      </c>
+      <c r="S59" s="16" t="s">
         <v>685</v>
       </c>
-      <c r="S59" s="16" t="s">
+      <c r="T59" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="U59" s="16" t="s">
         <v>686</v>
       </c>
-      <c r="T59" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="U59" s="16" t="s">
+      <c r="V59" s="16" t="s">
         <v>687</v>
       </c>
-      <c r="V59" s="16" t="s">
+      <c r="W59" s="16" t="s">
         <v>688</v>
       </c>
-      <c r="W59" s="16" t="s">
-        <v>689</v>
-      </c>
       <c r="X59" s="16" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="60" spans="1:24">
       <c r="A60" s="16" t="s">
+        <v>689</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>690</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="C60" s="16" t="s">
         <v>691</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="D60" s="16" t="s">
         <v>692</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="E60" s="16" t="s">
         <v>693</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="F60" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="16" t="s">
         <v>694</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>695</v>
       </c>
       <c r="H60" s="16">
         <v>9999</v>
@@ -8140,90 +8137,90 @@
         <v>65</v>
       </c>
       <c r="J60" s="16" t="s">
+        <v>695</v>
+      </c>
+      <c r="K60" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M60" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N60" s="22" t="s">
         <v>696</v>
-      </c>
-      <c r="K60" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L60" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M60" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="N60" s="22" t="s">
-        <v>697</v>
       </c>
       <c r="O60" s="12">
         <v>43625</v>
       </c>
       <c r="P60" s="12" t="s">
+        <v>697</v>
+      </c>
+      <c r="Q60" s="16" t="s">
         <v>698</v>
       </c>
-      <c r="Q60" s="16" t="s">
+      <c r="R60" s="16" t="s">
         <v>699</v>
       </c>
-      <c r="R60" s="16" t="s">
+      <c r="S60" s="16" t="s">
         <v>700</v>
       </c>
-      <c r="S60" s="16" t="s">
+      <c r="T60" s="16" t="s">
         <v>701</v>
       </c>
-      <c r="T60" s="16" t="s">
+      <c r="U60" s="16" t="s">
         <v>702</v>
-      </c>
-      <c r="U60" s="16" t="s">
-        <v>703</v>
       </c>
       <c r="V60" s="16">
         <v>9999</v>
       </c>
       <c r="W60" s="16" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="X60" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="61" spans="1:24">
       <c r="A61" s="30" t="s">
+        <v>704</v>
+      </c>
+      <c r="B61" s="16" t="s">
         <v>705</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="C61" s="16" t="s">
         <v>706</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="D61" s="16" t="s">
         <v>707</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="E61" s="16" t="s">
         <v>708</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="F61" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H61" s="16" t="s">
         <v>709</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H61" s="16" t="s">
+      <c r="I61" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J61" s="16" t="s">
         <v>710</v>
       </c>
-      <c r="I61" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J61" s="16" t="s">
+      <c r="K61" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L61" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M61" s="16" t="s">
         <v>711</v>
-      </c>
-      <c r="K61" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L61" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M61" s="16" t="s">
-        <v>712</v>
       </c>
       <c r="N61" s="22">
         <v>38626862120</v>
@@ -8232,152 +8229,152 @@
         <v>43079</v>
       </c>
       <c r="P61" s="12" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="Q61" s="16">
         <v>15</v>
       </c>
       <c r="R61" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="S61" s="16" t="s">
         <v>714</v>
       </c>
-      <c r="S61" s="16" t="s">
+      <c r="T61" s="16" t="s">
         <v>715</v>
       </c>
-      <c r="T61" s="16" t="s">
+      <c r="U61" s="16" t="s">
         <v>716</v>
       </c>
-      <c r="U61" s="16" t="s">
+      <c r="V61" s="16" t="s">
         <v>717</v>
       </c>
-      <c r="V61" s="16" t="s">
+      <c r="W61" s="16" t="s">
         <v>718</v>
       </c>
-      <c r="W61" s="16" t="s">
+      <c r="X61" s="16" t="s">
         <v>719</v>
-      </c>
-      <c r="X61" s="16" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="62" spans="1:24">
       <c r="A62" s="16" t="s">
+        <v>720</v>
+      </c>
+      <c r="B62" s="16" t="s">
         <v>721</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="C62" s="16" t="s">
         <v>722</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="D62" s="16" t="s">
         <v>723</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="E62" s="16" t="s">
         <v>724</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="F62" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J62" s="16" t="s">
         <v>725</v>
       </c>
-      <c r="F62" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I62" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J62" s="16" t="s">
+      <c r="K62" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L62" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M62" s="16" t="s">
         <v>726</v>
-      </c>
-      <c r="K62" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L62" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M62" s="16" t="s">
-        <v>727</v>
       </c>
       <c r="N62" s="22">
         <v>22954368529.639999</v>
       </c>
       <c r="O62" s="12" t="s">
+        <v>727</v>
+      </c>
+      <c r="P62" s="12" t="s">
         <v>728</v>
-      </c>
-      <c r="P62" s="12" t="s">
-        <v>729</v>
       </c>
       <c r="Q62" s="16">
         <v>11</v>
       </c>
       <c r="R62" s="16" t="s">
+        <v>729</v>
+      </c>
+      <c r="S62" s="16" t="s">
         <v>730</v>
       </c>
-      <c r="S62" s="16" t="s">
+      <c r="T62" s="16" t="s">
         <v>731</v>
       </c>
-      <c r="T62" s="16" t="s">
+      <c r="U62" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V62" s="16" t="s">
         <v>732</v>
       </c>
-      <c r="U62" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V62" s="16" t="s">
+      <c r="W62" s="16" t="s">
         <v>733</v>
       </c>
-      <c r="W62" s="16" t="s">
-        <v>734</v>
-      </c>
       <c r="X62" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="63" spans="1:24">
       <c r="A63" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B63" s="16" t="s">
         <v>735</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="C63" s="16" t="s">
         <v>736</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="D63" s="16" t="s">
         <v>737</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="E63" s="16" t="s">
         <v>738</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="F63" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H63" s="16" t="s">
         <v>739</v>
       </c>
-      <c r="F63" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H63" s="16" t="s">
-        <v>740</v>
-      </c>
       <c r="I63" s="16" t="s">
         <v>29</v>
       </c>
       <c r="J63" s="16" t="s">
+        <v>725</v>
+      </c>
+      <c r="K63" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L63" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M63" s="16" t="s">
         <v>726</v>
-      </c>
-      <c r="K63" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L63" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M63" s="16" t="s">
-        <v>727</v>
       </c>
       <c r="N63" s="22">
         <v>10920880573</v>
       </c>
       <c r="O63" s="12" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="P63" s="12" t="s">
         <v>85</v>
@@ -8386,57 +8383,57 @@
         <v>8</v>
       </c>
       <c r="R63" s="16" t="s">
+        <v>741</v>
+      </c>
+      <c r="S63" s="16" t="s">
+        <v>730</v>
+      </c>
+      <c r="T63" s="16" t="s">
         <v>742</v>
       </c>
-      <c r="S63" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="T63" s="16" t="s">
+      <c r="U63" s="16" t="s">
         <v>743</v>
       </c>
-      <c r="U63" s="16" t="s">
+      <c r="V63" s="16" t="s">
+        <v>732</v>
+      </c>
+      <c r="W63" s="16" t="s">
         <v>744</v>
       </c>
-      <c r="V63" s="16" t="s">
-        <v>733</v>
-      </c>
-      <c r="W63" s="16" t="s">
-        <v>745</v>
-      </c>
       <c r="X63" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="64" spans="1:24">
       <c r="A64" s="16" t="s">
+        <v>745</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>746</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="C64" s="16" t="s">
         <v>747</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="D64" s="16" t="s">
         <v>748</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="E64" s="16" t="s">
         <v>749</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="F64" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G64" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J64" s="16" t="s">
         <v>750</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G64" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J64" s="16" t="s">
-        <v>751</v>
       </c>
       <c r="K64" s="16" t="s">
         <v>52</v>
@@ -8460,57 +8457,57 @@
         <v>9999</v>
       </c>
       <c r="R64" s="16" t="s">
+        <v>751</v>
+      </c>
+      <c r="S64" s="16" t="s">
         <v>752</v>
       </c>
-      <c r="S64" s="16" t="s">
+      <c r="T64" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="U64" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V64" s="16" t="s">
         <v>753</v>
       </c>
-      <c r="T64" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="U64" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V64" s="16" t="s">
+      <c r="W64" s="16" t="s">
         <v>754</v>
       </c>
-      <c r="W64" s="16" t="s">
-        <v>755</v>
-      </c>
       <c r="X64" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="65" spans="1:24">
       <c r="A65" s="16" t="s">
+        <v>755</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>756</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="C65" s="16" t="s">
         <v>757</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="D65" s="16" t="s">
         <v>758</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="E65" s="16" t="s">
         <v>759</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="F65" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G65" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H65" s="16" t="s">
         <v>760</v>
       </c>
-      <c r="F65" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H65" s="16" t="s">
+      <c r="I65" s="16" t="s">
         <v>761</v>
       </c>
-      <c r="I65" s="16" t="s">
+      <c r="J65" s="16" t="s">
         <v>762</v>
-      </c>
-      <c r="J65" s="16" t="s">
-        <v>763</v>
       </c>
       <c r="K65" s="16" t="s">
         <v>52</v>
@@ -8525,66 +8522,66 @@
         <v>21503897914</v>
       </c>
       <c r="O65" s="12" t="s">
+        <v>763</v>
+      </c>
+      <c r="P65" s="12" t="s">
         <v>764</v>
-      </c>
-      <c r="P65" s="12" t="s">
-        <v>765</v>
       </c>
       <c r="Q65" s="16">
         <v>17.5</v>
       </c>
       <c r="R65" s="16" t="s">
+        <v>765</v>
+      </c>
+      <c r="S65" s="16" t="s">
+        <v>730</v>
+      </c>
+      <c r="T65" s="16" t="s">
         <v>766</v>
       </c>
-      <c r="S65" s="16" t="s">
-        <v>731</v>
-      </c>
-      <c r="T65" s="16" t="s">
+      <c r="U65" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V65" s="16" t="s">
         <v>767</v>
       </c>
-      <c r="U65" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V65" s="16" t="s">
+      <c r="W65" s="16" t="s">
         <v>768</v>
       </c>
-      <c r="W65" s="16" t="s">
-        <v>769</v>
-      </c>
       <c r="X65" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="66" spans="1:24">
       <c r="A66" s="16" t="s">
+        <v>769</v>
+      </c>
+      <c r="B66" s="16" t="s">
         <v>770</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="C66" s="16" t="s">
         <v>771</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="D66" s="16" t="s">
         <v>772</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="E66" s="16" t="s">
         <v>773</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="F66" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H66" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I66" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66" s="16" t="s">
         <v>774</v>
-      </c>
-      <c r="F66" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H66" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I66" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J66" s="16" t="s">
-        <v>775</v>
       </c>
       <c r="K66" s="16" t="s">
         <v>52</v>
@@ -8599,66 +8596,66 @@
         <v>32455048148</v>
       </c>
       <c r="O66" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="P66" s="12" t="s">
         <v>776</v>
-      </c>
-      <c r="P66" s="12" t="s">
-        <v>777</v>
       </c>
       <c r="Q66" s="16">
         <v>24</v>
       </c>
       <c r="R66" s="16" t="s">
+        <v>777</v>
+      </c>
+      <c r="S66" s="16" t="s">
+        <v>752</v>
+      </c>
+      <c r="T66" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="U66" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V66" s="16" t="s">
         <v>778</v>
       </c>
-      <c r="S66" s="16" t="s">
-        <v>753</v>
-      </c>
-      <c r="T66" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="U66" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V66" s="16" t="s">
+      <c r="W66" s="16" t="s">
         <v>779</v>
       </c>
-      <c r="W66" s="16" t="s">
-        <v>780</v>
-      </c>
       <c r="X66" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="67" spans="1:24">
       <c r="A67" s="16" t="s">
+        <v>780</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>781</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="C67" s="16" t="s">
         <v>782</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="D67" s="16" t="s">
         <v>783</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="E67" s="16" t="s">
         <v>784</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="F67" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I67" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" s="16" t="s">
         <v>785</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J67" s="16" t="s">
-        <v>786</v>
       </c>
       <c r="K67" s="16" t="s">
         <v>52</v>
@@ -8676,63 +8673,63 @@
         <v>41189</v>
       </c>
       <c r="P67" s="12" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="Q67" s="16">
         <v>13</v>
       </c>
       <c r="R67" s="16" t="s">
+        <v>787</v>
+      </c>
+      <c r="S67" s="16" t="s">
         <v>788</v>
-      </c>
-      <c r="S67" s="16" t="s">
-        <v>789</v>
       </c>
       <c r="T67" s="16">
         <v>219</v>
       </c>
       <c r="U67" s="16" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V67" s="16" t="s">
+        <v>789</v>
+      </c>
+      <c r="W67" s="16" t="s">
         <v>790</v>
       </c>
-      <c r="W67" s="16" t="s">
-        <v>791</v>
-      </c>
       <c r="X67" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="68" spans="1:24">
       <c r="A68" s="16" t="s">
+        <v>791</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>792</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="C68" s="16" t="s">
         <v>793</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="D68" s="16" t="s">
         <v>794</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="E68" s="16" t="s">
         <v>795</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="F68" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I68" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" s="16" t="s">
         <v>796</v>
-      </c>
-      <c r="F68" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I68" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J68" s="16" t="s">
-        <v>797</v>
       </c>
       <c r="K68" s="16" t="s">
         <v>52</v>
@@ -8756,131 +8753,131 @@
         <v>12</v>
       </c>
       <c r="R68" s="16" t="s">
+        <v>797</v>
+      </c>
+      <c r="S68" s="16" t="s">
         <v>798</v>
       </c>
-      <c r="S68" s="16" t="s">
+      <c r="T68" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="U68" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V68" s="16" t="s">
         <v>799</v>
       </c>
-      <c r="T68" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="U68" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V68" s="16" t="s">
+      <c r="W68" s="16" t="s">
         <v>800</v>
       </c>
-      <c r="W68" s="16" t="s">
-        <v>801</v>
-      </c>
       <c r="X68" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="69" spans="1:24" ht="15" customHeight="1">
       <c r="A69" s="16" t="s">
+        <v>801</v>
+      </c>
+      <c r="B69" s="16" t="s">
         <v>802</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="C69" s="29" t="s">
         <v>803</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="D69" s="16" t="s">
         <v>804</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="E69" s="16" t="s">
         <v>805</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="F69" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H69" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I69" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" s="16" t="s">
+        <v>796</v>
+      </c>
+      <c r="K69" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L69" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M69" s="16" t="s">
         <v>806</v>
-      </c>
-      <c r="F69" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H69" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I69" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J69" s="16" t="s">
-        <v>797</v>
-      </c>
-      <c r="K69" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L69" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="M69" s="16" t="s">
-        <v>807</v>
       </c>
       <c r="N69" s="22">
         <v>16886338370</v>
       </c>
       <c r="O69" s="12" t="s">
+        <v>807</v>
+      </c>
+      <c r="P69" s="12" t="s">
         <v>808</v>
-      </c>
-      <c r="P69" s="12" t="s">
-        <v>809</v>
       </c>
       <c r="Q69" s="16">
         <v>18</v>
       </c>
       <c r="R69" s="29" t="s">
+        <v>809</v>
+      </c>
+      <c r="S69" s="16" t="s">
         <v>810</v>
       </c>
-      <c r="S69" s="16" t="s">
+      <c r="T69" s="16" t="s">
         <v>811</v>
       </c>
-      <c r="T69" s="16" t="s">
+      <c r="U69" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V69" s="29" t="s">
         <v>812</v>
       </c>
-      <c r="U69" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V69" s="29" t="s">
+      <c r="W69" s="16" t="s">
         <v>813</v>
       </c>
-      <c r="W69" s="16" t="s">
+      <c r="X69" s="29" t="s">
         <v>814</v>
-      </c>
-      <c r="X69" s="29" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="70" spans="1:24">
       <c r="A70" s="16" t="s">
+        <v>815</v>
+      </c>
+      <c r="B70" s="16" t="s">
         <v>816</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="C70" s="16" t="s">
         <v>817</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="D70" s="16" t="s">
         <v>818</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="E70" s="16" t="s">
         <v>819</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="F70" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G70" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H70" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I70" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" s="16" t="s">
         <v>820</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G70" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I70" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J70" s="16" t="s">
-        <v>821</v>
       </c>
       <c r="K70" s="16" t="s">
         <v>52</v>
@@ -8895,81 +8892,81 @@
         <v>16782892881</v>
       </c>
       <c r="O70" s="12" t="s">
+        <v>821</v>
+      </c>
+      <c r="P70" s="12" t="s">
         <v>822</v>
-      </c>
-      <c r="P70" s="12" t="s">
-        <v>823</v>
       </c>
       <c r="Q70" s="16">
         <v>15</v>
       </c>
       <c r="R70" s="16" t="s">
+        <v>823</v>
+      </c>
+      <c r="S70" s="16" t="s">
         <v>824</v>
       </c>
-      <c r="S70" s="16" t="s">
+      <c r="T70" s="16" t="s">
         <v>825</v>
       </c>
-      <c r="T70" s="16" t="s">
+      <c r="U70" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V70" s="16" t="s">
         <v>826</v>
       </c>
-      <c r="U70" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V70" s="16" t="s">
+      <c r="W70" s="16" t="s">
         <v>827</v>
       </c>
-      <c r="W70" s="16" t="s">
-        <v>828</v>
-      </c>
       <c r="X70" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="71" spans="1:24">
       <c r="A71" s="16" t="s">
+        <v>828</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>829</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="C71" s="16" t="s">
         <v>830</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="D71" s="16" t="s">
         <v>831</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="E71" s="16" t="s">
         <v>832</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="F71" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I71" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" s="16" t="s">
         <v>833</v>
       </c>
-      <c r="F71" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G71" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J71" s="16" t="s">
+      <c r="K71" s="16" t="s">
         <v>834</v>
       </c>
-      <c r="K71" s="16" t="s">
+      <c r="L71" s="16" t="s">
         <v>835</v>
       </c>
-      <c r="L71" s="16" t="s">
+      <c r="M71" s="16" t="s">
         <v>836</v>
-      </c>
-      <c r="M71" s="16" t="s">
-        <v>837</v>
       </c>
       <c r="N71" s="22">
         <v>16864638530</v>
       </c>
       <c r="O71" s="12" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P71" s="12">
         <v>44350</v>
@@ -8978,58 +8975,58 @@
         <v>15</v>
       </c>
       <c r="R71" s="16" t="s">
+        <v>838</v>
+      </c>
+      <c r="S71" s="16" t="s">
         <v>839</v>
       </c>
-      <c r="S71" s="16" t="s">
+      <c r="T71" s="16" t="s">
         <v>840</v>
       </c>
-      <c r="T71" s="16" t="s">
+      <c r="U71" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V71" s="16" t="s">
         <v>841</v>
       </c>
-      <c r="U71" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V71" s="16" t="s">
+      <c r="W71" s="16" t="s">
         <v>842</v>
       </c>
-      <c r="W71" s="16" t="s">
-        <v>843</v>
-      </c>
       <c r="X71" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="72" spans="1:24">
       <c r="A72" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="B72" s="16" t="s">
         <v>844</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="C72" s="16" t="s">
         <v>845</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="D72" s="16" t="s">
         <v>846</v>
       </c>
-      <c r="D72" s="16" t="s">
+      <c r="E72" s="16" t="s">
         <v>847</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="F72" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G72" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I72" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J72" s="16" t="s">
         <v>848</v>
       </c>
-      <c r="F72" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G72" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I72" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J72" s="16" t="s">
-        <v>849</v>
-      </c>
       <c r="K72" s="16" t="s">
         <v>52</v>
       </c>
@@ -9037,13 +9034,13 @@
         <v>52</v>
       </c>
       <c r="M72" s="16" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="N72" s="22">
         <v>22270823688</v>
       </c>
       <c r="O72" s="12" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="P72" s="12">
         <v>44297</v>
@@ -9052,60 +9049,60 @@
         <v>15</v>
       </c>
       <c r="R72" s="16" t="s">
+        <v>850</v>
+      </c>
+      <c r="S72" s="16" t="s">
+        <v>798</v>
+      </c>
+      <c r="T72" s="16" t="s">
         <v>851</v>
       </c>
-      <c r="S72" s="16" t="s">
-        <v>799</v>
-      </c>
-      <c r="T72" s="16" t="s">
+      <c r="U72" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V72" s="16" t="s">
         <v>852</v>
       </c>
-      <c r="U72" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V72" s="16" t="s">
+      <c r="W72" s="16" t="s">
         <v>853</v>
       </c>
-      <c r="W72" s="16" t="s">
-        <v>854</v>
-      </c>
       <c r="X72" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="73" spans="1:24">
       <c r="A73" s="16" t="s">
+        <v>854</v>
+      </c>
+      <c r="B73" s="16" t="s">
         <v>855</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="C73" s="16" t="s">
         <v>856</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="D73" s="16" t="s">
         <v>857</v>
       </c>
-      <c r="D73" s="16" t="s">
+      <c r="E73" s="16" t="s">
         <v>858</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="F73" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G73" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I73" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J73" s="16" t="s">
         <v>859</v>
       </c>
-      <c r="F73" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="I73" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J73" s="16" t="s">
+      <c r="K73" s="16" t="s">
         <v>860</v>
-      </c>
-      <c r="K73" s="16" t="s">
-        <v>861</v>
       </c>
       <c r="L73" s="16" t="s">
         <v>52</v>
@@ -9117,48 +9114,48 @@
         <v>12341721000</v>
       </c>
       <c r="O73" s="12" t="s">
+        <v>861</v>
+      </c>
+      <c r="P73" s="12" t="s">
         <v>862</v>
-      </c>
-      <c r="P73" s="12" t="s">
-        <v>863</v>
       </c>
       <c r="Q73" s="16">
         <v>15</v>
       </c>
       <c r="R73" s="16" t="s">
+        <v>863</v>
+      </c>
+      <c r="S73" s="16" t="s">
+        <v>798</v>
+      </c>
+      <c r="T73" s="16" t="s">
         <v>864</v>
       </c>
-      <c r="S73" s="16" t="s">
-        <v>799</v>
-      </c>
-      <c r="T73" s="16" t="s">
+      <c r="U73" s="16" t="s">
+        <v>716</v>
+      </c>
+      <c r="V73" s="16" t="s">
+        <v>852</v>
+      </c>
+      <c r="W73" s="16" t="s">
         <v>865</v>
       </c>
-      <c r="U73" s="16" t="s">
-        <v>717</v>
-      </c>
-      <c r="V73" s="16" t="s">
-        <v>853</v>
-      </c>
-      <c r="W73" s="16" t="s">
-        <v>866</v>
-      </c>
       <c r="X73" s="16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="74" spans="1:24">
       <c r="A74" s="16" t="s">
+        <v>866</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>867</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="C74" s="16" t="s">
         <v>868</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="D74" s="16" t="s">
         <v>869</v>
-      </c>
-      <c r="D74" s="16" t="s">
-        <v>870</v>
       </c>
       <c r="E74" s="16" t="s">
         <v>52</v>
@@ -9200,22 +9197,22 @@
         <v>9999</v>
       </c>
       <c r="R74" s="16" t="s">
+        <v>870</v>
+      </c>
+      <c r="S74" s="16" t="s">
         <v>871</v>
       </c>
-      <c r="S74" s="16" t="s">
+      <c r="T74" s="16" t="s">
         <v>872</v>
       </c>
-      <c r="T74" s="16" t="s">
+      <c r="U74" s="16" t="s">
         <v>873</v>
       </c>
-      <c r="U74" s="16" t="s">
+      <c r="V74" s="16" t="s">
         <v>874</v>
       </c>
-      <c r="V74" s="16" t="s">
+      <c r="W74" s="16" t="s">
         <v>875</v>
-      </c>
-      <c r="W74" s="16" t="s">
-        <v>876</v>
       </c>
       <c r="X74" s="16" t="s">
         <v>102</v>
@@ -9223,16 +9220,16 @@
     </row>
     <row r="75" spans="1:24">
       <c r="A75" s="16" t="s">
+        <v>876</v>
+      </c>
+      <c r="B75" s="16" t="s">
         <v>877</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="C75" s="16" t="s">
         <v>878</v>
       </c>
-      <c r="C75" s="16" t="s">
+      <c r="D75" s="16" t="s">
         <v>879</v>
-      </c>
-      <c r="D75" s="16" t="s">
-        <v>880</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>52</v>
@@ -9274,22 +9271,22 @@
         <v>9999</v>
       </c>
       <c r="R75" s="16" t="s">
+        <v>880</v>
+      </c>
+      <c r="S75" s="16" t="s">
         <v>881</v>
       </c>
-      <c r="S75" s="16" t="s">
+      <c r="T75" s="16" t="s">
         <v>882</v>
       </c>
-      <c r="T75" s="16" t="s">
+      <c r="U75" s="16" t="s">
         <v>883</v>
       </c>
-      <c r="U75" s="16" t="s">
+      <c r="V75" s="16" t="s">
         <v>884</v>
       </c>
-      <c r="V75" s="16" t="s">
+      <c r="W75" s="16" t="s">
         <v>885</v>
-      </c>
-      <c r="W75" s="16" t="s">
-        <v>886</v>
       </c>
       <c r="X75" s="16" t="s">
         <v>102</v>
@@ -9297,10 +9294,10 @@
     </row>
     <row r="76" spans="1:24">
       <c r="A76" s="16" t="s">
+        <v>886</v>
+      </c>
+      <c r="B76" s="16" t="s">
         <v>887</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>888</v>
       </c>
       <c r="C76" s="16" t="s">
         <v>52</v>
@@ -9348,57 +9345,57 @@
         <v>9999</v>
       </c>
       <c r="R76" s="16" t="s">
+        <v>888</v>
+      </c>
+      <c r="S76" s="16" t="s">
         <v>889</v>
       </c>
-      <c r="S76" s="16" t="s">
+      <c r="T76" s="16" t="s">
         <v>890</v>
       </c>
-      <c r="T76" s="16" t="s">
+      <c r="U76" s="16" t="s">
         <v>891</v>
       </c>
-      <c r="U76" s="16" t="s">
+      <c r="V76" s="16" t="s">
         <v>892</v>
       </c>
-      <c r="V76" s="16" t="s">
+      <c r="W76" s="16" t="s">
         <v>893</v>
       </c>
-      <c r="W76" s="16" t="s">
-        <v>894</v>
-      </c>
       <c r="X76" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77" spans="1:24" s="34" customFormat="1">
       <c r="A77" s="31" t="s">
+        <v>894</v>
+      </c>
+      <c r="B77" s="31" t="s">
         <v>895</v>
       </c>
-      <c r="B77" s="31" t="s">
+      <c r="C77" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F77" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G77" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H77" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I77" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="J77" s="31" t="s">
         <v>896</v>
-      </c>
-      <c r="C77" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D77" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E77" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="F77" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G77" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="H77" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="I77" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="J77" s="31" t="s">
-        <v>897</v>
       </c>
       <c r="K77" s="31" t="s">
         <v>52</v>
@@ -9422,33 +9419,33 @@
         <v>9999</v>
       </c>
       <c r="R77" s="31" t="s">
+        <v>897</v>
+      </c>
+      <c r="S77" s="31" t="s">
         <v>898</v>
       </c>
-      <c r="S77" s="31" t="s">
+      <c r="T77" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="U77" s="31" t="s">
         <v>899</v>
       </c>
-      <c r="T77" s="31" t="s">
-        <v>329</v>
-      </c>
-      <c r="U77" s="31" t="s">
+      <c r="V77" s="31" t="s">
         <v>900</v>
       </c>
-      <c r="V77" s="31" t="s">
+      <c r="W77" s="31" t="s">
         <v>901</v>
       </c>
-      <c r="W77" s="31" t="s">
-        <v>902</v>
-      </c>
       <c r="X77" s="31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:24" s="34" customFormat="1">
       <c r="A78" s="31" t="s">
+        <v>902</v>
+      </c>
+      <c r="B78" s="31" t="s">
         <v>903</v>
-      </c>
-      <c r="B78" s="31" t="s">
-        <v>904</v>
       </c>
       <c r="C78" s="31" t="s">
         <v>52</v>
@@ -9496,39 +9493,39 @@
         <v>9999</v>
       </c>
       <c r="R78" s="31" t="s">
+        <v>904</v>
+      </c>
+      <c r="S78" s="31" t="s">
         <v>905</v>
       </c>
-      <c r="S78" s="31" t="s">
+      <c r="T78" s="31" t="s">
+        <v>905</v>
+      </c>
+      <c r="U78" s="31" t="s">
         <v>906</v>
       </c>
-      <c r="T78" s="31" t="s">
-        <v>906</v>
-      </c>
-      <c r="U78" s="31" t="s">
+      <c r="V78" s="31" t="s">
         <v>907</v>
       </c>
-      <c r="V78" s="31" t="s">
+      <c r="W78" s="31" t="s">
         <v>908</v>
       </c>
-      <c r="W78" s="31" t="s">
-        <v>909</v>
-      </c>
       <c r="X78" s="31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="79" spans="1:24" ht="15.75" customHeight="1">
       <c r="A79" s="16" t="s">
+        <v>909</v>
+      </c>
+      <c r="B79" s="16" t="s">
         <v>910</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="C79" s="16" t="s">
         <v>911</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="D79" s="16" t="s">
         <v>912</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>913</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>52</v>
@@ -9570,22 +9567,22 @@
         <v>9999</v>
       </c>
       <c r="R79" s="29" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="S79" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="T79" s="16" t="s">
         <v>98</v>
       </c>
       <c r="U79" s="16" t="s">
+        <v>914</v>
+      </c>
+      <c r="V79" s="16" t="s">
         <v>915</v>
       </c>
-      <c r="V79" s="16" t="s">
+      <c r="W79" s="16" t="s">
         <v>916</v>
-      </c>
-      <c r="W79" s="16" t="s">
-        <v>917</v>
       </c>
       <c r="X79" s="16" t="s">
         <v>102</v>
@@ -9593,13 +9590,13 @@
     </row>
     <row r="80" spans="1:24" ht="19.5" customHeight="1">
       <c r="A80" s="16" t="s">
+        <v>917</v>
+      </c>
+      <c r="B80" s="16" t="s">
         <v>918</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="C80" s="29" t="s">
         <v>919</v>
-      </c>
-      <c r="C80" s="29" t="s">
-        <v>920</v>
       </c>
       <c r="D80" s="16" t="s">
         <v>52</v>
@@ -9644,22 +9641,22 @@
         <v>9999</v>
       </c>
       <c r="R80" s="29" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="S80" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="T80" s="16" t="s">
         <v>98</v>
       </c>
       <c r="U80" s="16" t="s">
+        <v>921</v>
+      </c>
+      <c r="V80" s="16" t="s">
         <v>922</v>
       </c>
-      <c r="V80" s="16" t="s">
+      <c r="W80" s="16" t="s">
         <v>923</v>
-      </c>
-      <c r="W80" s="16" t="s">
-        <v>924</v>
       </c>
       <c r="X80" s="16" t="s">
         <v>102</v>
@@ -9667,25 +9664,25 @@
     </row>
     <row r="81" spans="1:24">
       <c r="A81" s="16" t="s">
+        <v>924</v>
+      </c>
+      <c r="B81" s="16" t="s">
         <v>925</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="C81" s="16" t="s">
         <v>926</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="D81" s="16" t="s">
         <v>927</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="E81" s="16" t="s">
         <v>928</v>
       </c>
-      <c r="E81" s="16" t="s">
-        <v>929</v>
-      </c>
       <c r="F81" s="16" t="s">
         <v>29</v>
       </c>
       <c r="G81" s="16" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="H81" s="16" t="s">
         <v>52</v>
@@ -9697,7 +9694,7 @@
         <v>50</v>
       </c>
       <c r="K81" s="16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="L81" s="16" t="s">
         <v>52</v>
@@ -9718,57 +9715,57 @@
         <v>9999</v>
       </c>
       <c r="R81" s="16" t="s">
+        <v>929</v>
+      </c>
+      <c r="S81" s="16" t="s">
+        <v>898</v>
+      </c>
+      <c r="T81" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="U81" s="16" t="s">
         <v>930</v>
       </c>
-      <c r="S81" s="16" t="s">
-        <v>899</v>
-      </c>
-      <c r="T81" s="16" t="s">
-        <v>329</v>
-      </c>
-      <c r="U81" s="16" t="s">
+      <c r="V81" s="16" t="s">
         <v>931</v>
       </c>
-      <c r="V81" s="16" t="s">
+      <c r="W81" s="16" t="s">
         <v>932</v>
       </c>
-      <c r="W81" s="16" t="s">
-        <v>933</v>
-      </c>
       <c r="X81" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="82" spans="1:24">
       <c r="A82" s="16" t="s">
+        <v>933</v>
+      </c>
+      <c r="B82" s="16" t="s">
         <v>934</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="C82" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="16" t="s">
         <v>935</v>
       </c>
-      <c r="C82" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D82" s="16" t="s">
+      <c r="E82" s="16" t="s">
         <v>936</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="F82" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="16" t="s">
+        <v>936</v>
+      </c>
+      <c r="H82" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I82" s="16" t="s">
         <v>937</v>
       </c>
-      <c r="F82" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G82" s="16" t="s">
-        <v>937</v>
-      </c>
-      <c r="H82" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I82" s="16" t="s">
-        <v>938</v>
-      </c>
       <c r="J82" s="16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="K82" s="16" t="s">
         <v>50</v>
@@ -9792,60 +9789,60 @@
         <v>9999</v>
       </c>
       <c r="R82" s="16" t="s">
+        <v>938</v>
+      </c>
+      <c r="S82" s="16" t="s">
+        <v>898</v>
+      </c>
+      <c r="T82" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="U82" s="16" t="s">
         <v>939</v>
       </c>
-      <c r="S82" s="16" t="s">
-        <v>899</v>
-      </c>
-      <c r="T82" s="16" t="s">
-        <v>329</v>
-      </c>
-      <c r="U82" s="16" t="s">
+      <c r="V82" s="16" t="s">
         <v>940</v>
       </c>
-      <c r="V82" s="16" t="s">
+      <c r="W82" s="16" t="s">
         <v>941</v>
       </c>
-      <c r="W82" s="16" t="s">
-        <v>942</v>
-      </c>
       <c r="X82" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="83" spans="1:24">
       <c r="A83" s="16" t="s">
+        <v>942</v>
+      </c>
+      <c r="B83" s="16" t="s">
         <v>943</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="C83" s="16" t="s">
         <v>944</v>
       </c>
-      <c r="C83" s="16" t="s">
+      <c r="D83" s="16" t="s">
         <v>945</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="E83" s="16" t="s">
         <v>946</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="F83" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="16" t="s">
         <v>947</v>
       </c>
-      <c r="F83" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G83" s="16" t="s">
+      <c r="H83" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I83" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J83" s="16" t="s">
+        <v>896</v>
+      </c>
+      <c r="K83" s="16" t="s">
         <v>948</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I83" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J83" s="16" t="s">
-        <v>897</v>
-      </c>
-      <c r="K83" s="16" t="s">
-        <v>949</v>
       </c>
       <c r="L83" s="16" t="s">
         <v>52</v>
@@ -9866,25 +9863,25 @@
         <v>9999</v>
       </c>
       <c r="R83" s="16" t="s">
+        <v>949</v>
+      </c>
+      <c r="S83" s="16" t="s">
         <v>950</v>
       </c>
-      <c r="S83" s="16" t="s">
+      <c r="T83" s="16" t="s">
         <v>951</v>
       </c>
-      <c r="T83" s="16" t="s">
+      <c r="U83" s="16" t="s">
+        <v>930</v>
+      </c>
+      <c r="V83" s="16" t="s">
         <v>952</v>
       </c>
-      <c r="U83" s="16" t="s">
-        <v>931</v>
-      </c>
-      <c r="V83" s="16" t="s">
+      <c r="W83" s="16" t="s">
         <v>953</v>
       </c>
-      <c r="W83" s="16" t="s">
-        <v>954</v>
-      </c>
       <c r="X83" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>